<commit_message>
Computed the numbers of parameters for the kaggle submission
</commit_message>
<xml_diff>
--- a/kaggle/parameters_calculator.xlsx
+++ b/kaggle/parameters_calculator.xlsx
@@ -8,7 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Aditya" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Kaggle Feb3" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Aditya" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t xml:space="preserve">Size</t>
   </si>
@@ -47,6 +48,9 @@
   </si>
   <si>
     <t xml:space="preserve">Parameter Size (Bytes)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model Size (bytes)</t>
   </si>
   <si>
     <t xml:space="preserve">Model Size</t>
@@ -64,6 +68,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -85,6 +90,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -129,8 +135,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -155,221 +165,534 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.42"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
-        <v>3</v>
-      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>96</v>
-      </c>
-      <c r="D2" s="0" t="n">
+      <c r="A2" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <f aca="false">(A2*A2*B2+1)*C2</f>
+        <v>2688</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <f aca="false">(A3*A3*B3+1)*C3</f>
+        <v>83040</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <f aca="false">(A4*A4*B4+1)*C4</f>
+        <v>83040</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>192</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <f aca="false">(A5*A5*B5+1)*C5</f>
+        <v>166080</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>192</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>192</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <f aca="false">(A6*A6*B6+1)*C6</f>
+        <v>331968</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>192</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>192</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <f aca="false">(A7*A7*B7+1)*C7</f>
+        <v>331968</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="2" t="n">
+        <f aca="false">SUM(D2:D8)</f>
+        <v>998784</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
+        <f aca="false">12*12*192</f>
+        <v>27648</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1" t="n">
+        <f aca="false">A12*B12</f>
+        <v>276480</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="2" t="n">
+        <f aca="false">SUM(D12:D13)</f>
+        <v>276480</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1" t="n">
+        <f aca="false">D14+D9</f>
+        <v>1275264</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1" t="n">
+        <f aca="false">4</f>
+        <v>4</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1" t="n">
+        <f aca="false">D17*D16</f>
+        <v>5101056</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1" t="n">
+        <f aca="false">G16/G17</f>
+        <v>26</v>
+      </c>
+      <c r="H18" s="1"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G18"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.3"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="1" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="D2" s="1" t="n">
         <f aca="false">A2*A2*B2*C2</f>
         <v>2592</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>96</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>96</v>
-      </c>
-      <c r="D3" s="0" t="n">
+      <c r="A3" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="D3" s="1" t="n">
         <f aca="false">A3*A3*B3*C3</f>
         <v>82944</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>96</v>
-      </c>
-      <c r="C4" s="0" t="n">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="C4" s="1" t="n">
         <v>256</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <f aca="false">A4*A4*B4*C4</f>
         <v>221184</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>96</v>
-      </c>
-      <c r="C5" s="0" t="n">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="C5" s="1" t="n">
         <v>256</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <f aca="false">A5*A5*B5*C5</f>
         <v>221184</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B6" s="0" t="n">
+      <c r="A6" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="n">
         <v>256</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <v>256</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <f aca="false">A6*A6*B6*C6</f>
         <v>589824</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B7" s="0" t="n">
+      <c r="A7" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="n">
         <v>256</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="1" t="n">
         <v>512</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <f aca="false">A7*A7*B7*C7</f>
         <v>1179648</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B8" s="0" t="n">
+      <c r="A8" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1" t="n">
         <v>512</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="1" t="n">
         <v>512</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <f aca="false">A8*A8*B8*C8</f>
         <v>2359296</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D9" s="1" t="n">
+      <c r="D9" s="2" t="n">
         <f aca="false">SUM(D2:D8)</f>
         <v>4656672</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+      <c r="A12" s="1" t="n">
         <f aca="false">4*4*1024</f>
         <v>16384</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="1" t="n">
         <f aca="false">A12*B12</f>
         <v>16384000</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+      <c r="A13" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="1" t="n">
         <f aca="false">A13*B13</f>
         <v>10000</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D14" s="1" t="n">
+      <c r="D14" s="2" t="n">
         <f aca="false">SUM(D12:D13)</f>
         <v>16394000</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="1" t="n">
         <f aca="false">D14+D9</f>
         <v>21050672</v>
       </c>
-      <c r="G16" s="0" t="n">
+      <c r="G16" s="1" t="n">
         <v>104</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="D17" s="1" t="n">
         <f aca="false">4</f>
         <v>4</v>
       </c>
-      <c r="G17" s="0" t="n">
+      <c r="G17" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="0" t="n">
+      <c r="B18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="1" t="n">
         <f aca="false">D17*D16</f>
         <v>84202688</v>
       </c>
-      <c r="G18" s="0" t="n">
+      <c r="G18" s="1" t="n">
         <f aca="false">G16/G17</f>
         <v>26</v>
       </c>

</xml_diff>